<commit_message>
DS_Algo almost final version
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/xldata.xlsx
+++ b/src/test/resources/exceldata/xldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha\OneDrive\Documents\GitHub\Projects\Proj-DS-ALGO\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867C842A-8657-4003-B977-65EB04AC6997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B31743A-905F-4F99-B1A4-A8DDFAE37B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>pythonCode</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>print("I am from Implementation of BST")</t>
+  </si>
+  <si>
+    <t>print("I am from Graph link")</t>
+  </si>
+  <si>
+    <t>print("I am from Graph Representation")</t>
   </si>
 </sst>
 </file>
@@ -476,9 +482,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -486,7 +492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -501,177 +507,187 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B49163-7997-4684-9053-6FF2C716D75B}">
-  <dimension ref="A1:A33"/>
+  <dimension ref="A1:A35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>